<commit_message>
fix: resolve mask xarray spatial dims
</commit_message>
<xml_diff>
--- a/notebooks/data_ns/CORINE_LAND_COVER_MONTPELLIER.xlsx
+++ b/notebooks/data_ns/CORINE_LAND_COVER_MONTPELLIER.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael_belluau\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaetan/Code/projets/_NaturalSolutions/_Ecoteka/3m-ai/01-data-preparation/notebooks/data_ns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E34FF7-50EE-4796-AE3A-6DFB8004A050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DBDD78-DE12-3D4A-975C-01DE1D97743D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{837D7804-A0DA-4326-9260-55DD034E7173}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20500" xr2:uid="{837D7804-A0DA-4326-9260-55DD034E7173}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$G$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$H$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="153">
   <si>
     <t>c2021_niv1</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>H5.3</t>
+  </si>
+  <si>
+    <t>eunis_niv1_label</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,22 +862,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF824820-C93B-43E1-A10F-EB638DB4C8ED}">
-  <dimension ref="A1:G81"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="8" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,13 +897,16 @@
         <v>92</v>
       </c>
       <c r="F1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -914,12 +922,15 @@
       <c r="E2" t="s">
         <v>95</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -935,14 +946,17 @@
       <c r="E3" t="s">
         <v>95</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>103</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -958,12 +972,15 @@
       <c r="E4" t="s">
         <v>95</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -979,14 +996,17 @@
       <c r="E5" t="s">
         <v>95</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
         <v>103</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1002,12 +1022,15 @@
       <c r="E6" t="s">
         <v>95</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1023,14 +1046,17 @@
       <c r="E7" t="s">
         <v>95</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
         <v>103</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1046,12 +1072,15 @@
       <c r="E8" t="s">
         <v>95</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1067,14 +1096,17 @@
       <c r="E9" t="s">
         <v>95</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
         <v>103</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1090,12 +1122,15 @@
       <c r="E10" t="s">
         <v>95</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>101</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1111,14 +1146,17 @@
       <c r="E11" t="s">
         <v>95</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
         <v>103</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1134,14 +1172,17 @@
       <c r="E12" t="s">
         <v>95</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
         <v>102</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1157,14 +1198,17 @@
       <c r="E13" t="s">
         <v>95</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
         <v>103</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1177,13 +1221,16 @@
       <c r="D14" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="1"/>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1199,14 +1246,17 @@
       <c r="E15" t="s">
         <v>95</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
         <v>103</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1222,14 +1272,17 @@
       <c r="E16" t="s">
         <v>95</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
         <v>101</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1245,14 +1298,17 @@
       <c r="E17" t="s">
         <v>95</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
         <v>103</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1268,14 +1324,17 @@
       <c r="E18" t="s">
         <v>95</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
         <v>101</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1291,14 +1350,17 @@
       <c r="E19" t="s">
         <v>95</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
         <v>103</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1314,14 +1376,17 @@
       <c r="E20" t="s">
         <v>95</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
         <v>101</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1337,14 +1402,17 @@
       <c r="E21" t="s">
         <v>95</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
         <v>103</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1360,14 +1428,17 @@
       <c r="E22" t="s">
         <v>95</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
         <v>102</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1383,14 +1454,17 @@
       <c r="E23" t="s">
         <v>95</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
         <v>103</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1406,14 +1480,17 @@
       <c r="E24" t="s">
         <v>95</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
         <v>102</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1429,14 +1506,17 @@
       <c r="E25" t="s">
         <v>95</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="G25" t="s">
         <v>101</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1452,14 +1532,17 @@
       <c r="E26" t="s">
         <v>95</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
         <v>103</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1475,14 +1558,17 @@
       <c r="E27" t="s">
         <v>95</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="G27" t="s">
         <v>103</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1498,14 +1584,17 @@
       <c r="E28" t="s">
         <v>95</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28">
+        <v>9</v>
+      </c>
+      <c r="G28" t="s">
         <v>103</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1521,14 +1610,17 @@
       <c r="E29" t="s">
         <v>95</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
         <v>103</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1544,14 +1636,17 @@
       <c r="E30" t="s">
         <v>95</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="G30" t="s">
         <v>103</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1567,14 +1662,17 @@
       <c r="E31" t="s">
         <v>95</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
         <v>103</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1590,14 +1688,17 @@
       <c r="E32" t="s">
         <v>95</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
         <v>103</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1613,14 +1714,17 @@
       <c r="E33" t="s">
         <v>95</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33">
+        <v>9</v>
+      </c>
+      <c r="G33" t="s">
         <v>103</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1636,14 +1740,17 @@
       <c r="E34" t="s">
         <v>95</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34">
+        <v>9</v>
+      </c>
+      <c r="G34" t="s">
         <v>113</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1659,14 +1766,17 @@
       <c r="E35" t="s">
         <v>95</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35">
+        <v>9</v>
+      </c>
+      <c r="G35" t="s">
         <v>103</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1682,14 +1792,17 @@
       <c r="E36" t="s">
         <v>95</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36">
+        <v>9</v>
+      </c>
+      <c r="G36" t="s">
         <v>116</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1705,14 +1818,17 @@
       <c r="E37" t="s">
         <v>95</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
         <v>103</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1728,14 +1844,17 @@
       <c r="E38" t="s">
         <v>95</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38">
+        <v>9</v>
+      </c>
+      <c r="G38" t="s">
         <v>101</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1751,14 +1870,17 @@
       <c r="E39" t="s">
         <v>95</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39">
+        <v>9</v>
+      </c>
+      <c r="G39" t="s">
         <v>103</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1774,12 +1896,15 @@
       <c r="E40" t="s">
         <v>110</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
         <v>119</v>
       </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1795,14 +1920,17 @@
       <c r="E41" t="s">
         <v>95</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
         <v>103</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1818,12 +1946,15 @@
       <c r="E42" t="s">
         <v>110</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="G42" t="s">
         <v>120</v>
       </c>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>4</v>
       </c>
@@ -1839,14 +1970,17 @@
       <c r="E43" t="s">
         <v>95</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43">
+        <v>9</v>
+      </c>
+      <c r="G43" t="s">
         <v>103</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4</v>
       </c>
@@ -1862,14 +1996,17 @@
       <c r="E44" t="s">
         <v>95</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44">
+        <v>9</v>
+      </c>
+      <c r="G44" t="s">
         <v>103</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>4</v>
       </c>
@@ -1885,14 +2022,17 @@
       <c r="E45" t="s">
         <v>95</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45">
+        <v>9</v>
+      </c>
+      <c r="G45" t="s">
         <v>103</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>4</v>
       </c>
@@ -1908,14 +2048,17 @@
       <c r="E46" t="s">
         <v>95</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46">
+        <v>9</v>
+      </c>
+      <c r="G46" t="s">
         <v>103</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -1931,12 +2074,15 @@
       <c r="E47" t="s">
         <v>110</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
         <v>109</v>
       </c>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1949,13 +2095,16 @@
       <c r="D48" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="1"/>
+      <c r="F48">
+        <v>8</v>
+      </c>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>5</v>
       </c>
@@ -1971,14 +2120,17 @@
       <c r="E49" t="s">
         <v>95</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49">
+        <v>9</v>
+      </c>
+      <c r="G49" t="s">
         <v>103</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>5</v>
       </c>
@@ -1994,12 +2146,15 @@
       <c r="E50" t="s">
         <v>96</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50">
+        <v>8</v>
+      </c>
+      <c r="G50" t="s">
         <v>118</v>
       </c>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2015,14 +2170,17 @@
       <c r="E51" t="s">
         <v>96</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51">
+        <v>8</v>
+      </c>
+      <c r="G51" t="s">
         <v>102</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2038,10 +2196,13 @@
       <c r="E52" t="s">
         <v>122</v>
       </c>
-      <c r="F52" s="1"/>
+      <c r="F52">
+        <v>4</v>
+      </c>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2057,14 +2218,17 @@
       <c r="E53" t="s">
         <v>127</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53">
+        <v>5</v>
+      </c>
+      <c r="G53" t="s">
         <v>143</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2080,14 +2244,17 @@
       <c r="E54" t="s">
         <v>127</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54">
+        <v>5</v>
+      </c>
+      <c r="G54" t="s">
         <v>143</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>5</v>
       </c>
@@ -2103,14 +2270,17 @@
       <c r="E55" t="s">
         <v>132</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55">
+        <v>6</v>
+      </c>
+      <c r="G55" t="s">
         <v>136</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5</v>
       </c>
@@ -2126,14 +2296,17 @@
       <c r="E56" t="s">
         <v>132</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56">
+        <v>6</v>
+      </c>
+      <c r="G56" t="s">
         <v>136</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>5</v>
       </c>
@@ -2149,14 +2322,17 @@
       <c r="E57" t="s">
         <v>132</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57">
+        <v>6</v>
+      </c>
+      <c r="G57" t="s">
         <v>138</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>5</v>
       </c>
@@ -2172,14 +2348,17 @@
       <c r="E58" t="s">
         <v>132</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58">
+        <v>6</v>
+      </c>
+      <c r="G58" t="s">
         <v>140</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>6</v>
       </c>
@@ -2195,12 +2374,15 @@
       <c r="E59" t="s">
         <v>132</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59">
+        <v>6</v>
+      </c>
+      <c r="G59" t="s">
         <v>136</v>
       </c>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>6</v>
       </c>
@@ -2216,14 +2398,17 @@
       <c r="E60" t="s">
         <v>132</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60">
+        <v>6</v>
+      </c>
+      <c r="G60" t="s">
         <v>136</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>6</v>
       </c>
@@ -2239,14 +2424,17 @@
       <c r="E61" t="s">
         <v>132</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61">
+        <v>6</v>
+      </c>
+      <c r="G61" t="s">
         <v>138</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>6</v>
       </c>
@@ -2262,12 +2450,15 @@
       <c r="E62" t="s">
         <v>132</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62">
+        <v>6</v>
+      </c>
+      <c r="G62" t="s">
         <v>140</v>
       </c>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>6</v>
       </c>
@@ -2283,10 +2474,13 @@
       <c r="E63" t="s">
         <v>132</v>
       </c>
-      <c r="F63" s="1"/>
+      <c r="F63">
+        <v>6</v>
+      </c>
       <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>6</v>
       </c>
@@ -2302,14 +2496,17 @@
       <c r="E64" t="s">
         <v>132</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64">
+        <v>6</v>
+      </c>
+      <c r="G64" t="s">
         <v>149</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>6</v>
       </c>
@@ -2325,14 +2522,17 @@
       <c r="E65" t="s">
         <v>132</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65">
+        <v>6</v>
+      </c>
+      <c r="G65" t="s">
         <v>133</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>6</v>
       </c>
@@ -2348,12 +2548,15 @@
       <c r="E66" t="s">
         <v>127</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66">
+        <v>5</v>
+      </c>
+      <c r="G66" t="s">
         <v>131</v>
       </c>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>6</v>
       </c>
@@ -2369,14 +2572,17 @@
       <c r="E67" t="s">
         <v>127</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67">
+        <v>5</v>
+      </c>
+      <c r="G67" t="s">
         <v>145</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>6</v>
       </c>
@@ -2392,14 +2598,17 @@
       <c r="E68" t="s">
         <v>132</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68">
+        <v>6</v>
+      </c>
+      <c r="G68" t="s">
         <v>133</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>7</v>
       </c>
@@ -2415,12 +2624,15 @@
       <c r="E69" t="s">
         <v>127</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69">
+        <v>5</v>
+      </c>
+      <c r="G69" t="s">
         <v>128</v>
       </c>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>7</v>
       </c>
@@ -2436,14 +2648,17 @@
       <c r="E70" t="s">
         <v>127</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70" t="s">
         <v>129</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>7</v>
       </c>
@@ -2459,14 +2674,17 @@
       <c r="E71" t="s">
         <v>127</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71" t="s">
         <v>126</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>7</v>
       </c>
@@ -2482,14 +2700,17 @@
       <c r="E72" t="s">
         <v>122</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72">
+        <v>4</v>
+      </c>
+      <c r="G72" t="s">
         <v>123</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>7</v>
       </c>
@@ -2505,14 +2726,17 @@
       <c r="E73" t="s">
         <v>97</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73">
+        <v>7</v>
+      </c>
+      <c r="G73" t="s">
         <v>150</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>7</v>
       </c>
@@ -2528,10 +2752,13 @@
       <c r="E74" t="s">
         <v>98</v>
       </c>
-      <c r="F74" s="1"/>
+      <c r="F74">
+        <v>2</v>
+      </c>
       <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>7</v>
       </c>
@@ -2547,10 +2774,13 @@
       <c r="E75" t="s">
         <v>99</v>
       </c>
-      <c r="F75" s="1"/>
+      <c r="F75">
+        <v>3</v>
+      </c>
       <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>7</v>
       </c>
@@ -2566,10 +2796,13 @@
       <c r="E76" t="s">
         <v>98</v>
       </c>
-      <c r="F76" s="1"/>
+      <c r="F76">
+        <v>2</v>
+      </c>
       <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>8</v>
       </c>
@@ -2585,10 +2818,13 @@
       <c r="E77" t="s">
         <v>99</v>
       </c>
-      <c r="F77" s="1"/>
+      <c r="F77">
+        <v>3</v>
+      </c>
       <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>8</v>
       </c>
@@ -2604,10 +2840,13 @@
       <c r="E78" t="s">
         <v>99</v>
       </c>
-      <c r="F78" s="1"/>
+      <c r="F78">
+        <v>3</v>
+      </c>
       <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>8</v>
       </c>
@@ -2623,10 +2862,13 @@
       <c r="E79" t="s">
         <v>99</v>
       </c>
-      <c r="F79" s="1"/>
+      <c r="F79">
+        <v>3</v>
+      </c>
       <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>8</v>
       </c>
@@ -2642,10 +2884,13 @@
       <c r="E80" t="s">
         <v>98</v>
       </c>
-      <c r="F80" s="1"/>
+      <c r="F80">
+        <v>2</v>
+      </c>
       <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>8</v>
       </c>
@@ -2661,11 +2906,20 @@
       <c r="E81" t="s">
         <v>100</v>
       </c>
-      <c r="F81" s="1"/>
+      <c r="F81">
+        <v>1</v>
+      </c>
       <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G81" xr:uid="{BF824820-C93B-43E1-A10F-EB638DB4C8ED}"/>
+  <autoFilter ref="A1:H81" xr:uid="{BF824820-C93B-43E1-A10F-EB638DB4C8ED}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="E"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>